<commit_message>
base finished chapter 8 90%
</commit_message>
<xml_diff>
--- a/autocrword/models/chapter_8/土建用量表.xlsx
+++ b/autocrword/models/chapter_8/土建用量表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\PycharmProjects\Odoo_addons_NB\autocrword\models\chapter_8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0350363E-8608-4021-B72C-B0EA6AECCDC5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BFAA18-E906-4363-9F54-346CEB75EAFF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="569" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="1080" windowWidth="19335" windowHeight="13830" tabRatio="569" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="成果输出" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="428">
   <si>
     <t>项目</t>
   </si>
@@ -1720,10 +1720,6 @@
     <t>浆砌石</t>
   </si>
   <si>
-    <t>架空线路</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>直埋电缆</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -2345,6 +2341,38 @@
   </si>
   <si>
     <t>{{合计亩_临时用地面积}}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>建筑面积</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>土石方开挖</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>浆砌石</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>风机机组</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>主变压器</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>土石方回填</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>混凝土</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢筋</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -4663,11 +4691,11 @@
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="145" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
@@ -4675,30 +4703,30 @@
     </row>
     <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="121" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" s="174" t="s">
         <v>311</v>
       </c>
-      <c r="B2" s="174" t="s">
+      <c r="C2" s="174" t="s">
         <v>312</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="D2" s="174" t="s">
         <v>313</v>
       </c>
-      <c r="D2" s="174" t="s">
+      <c r="E2" s="174" t="s">
         <v>314</v>
       </c>
-      <c r="E2" s="174" t="s">
+      <c r="F2" s="174" t="s">
         <v>315</v>
       </c>
-      <c r="F2" s="174" t="s">
+      <c r="G2" s="177" t="s">
         <v>316</v>
-      </c>
-      <c r="G2" s="177" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="178" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B3" s="175">
         <f>条件输入!B13</f>
@@ -4727,7 +4755,7 @@
     </row>
     <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="178" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B4" s="175">
         <f>条件输入!B14</f>
@@ -4756,7 +4784,7 @@
     </row>
     <row r="5" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="178" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B5" s="175">
         <f>条件输入!B15</f>
@@ -4785,7 +4813,7 @@
     </row>
     <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="178" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B6" s="175">
         <f>条件输入!B16</f>
@@ -4814,7 +4842,7 @@
     </row>
     <row r="7" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="178" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B7" s="175">
         <f>条件输入!B17</f>
@@ -4843,7 +4871,7 @@
     </row>
     <row r="8" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="180" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B8" s="176">
         <f>条件输入!B18</f>
@@ -4874,11 +4902,11 @@
     <row r="10" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="11" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="145" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
@@ -4886,40 +4914,40 @@
     </row>
     <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="121" t="s">
+        <v>325</v>
+      </c>
+      <c r="B12" s="174" t="s">
         <v>326</v>
       </c>
-      <c r="B12" s="174" t="s">
+      <c r="C12" s="174" t="s">
         <v>327</v>
       </c>
-      <c r="C12" s="174" t="s">
+      <c r="D12" s="174" t="s">
+        <v>340</v>
+      </c>
+      <c r="E12" s="174" t="s">
         <v>328</v>
       </c>
-      <c r="D12" s="174" t="s">
-        <v>341</v>
-      </c>
-      <c r="E12" s="174" t="s">
+      <c r="F12" s="174" t="s">
         <v>329</v>
       </c>
-      <c r="F12" s="174" t="s">
+      <c r="G12" s="174" t="s">
         <v>330</v>
       </c>
-      <c r="G12" s="174" t="s">
+      <c r="H12" s="174" t="s">
         <v>331</v>
       </c>
-      <c r="H12" s="174" t="s">
+      <c r="I12" s="174" t="s">
         <v>332</v>
       </c>
-      <c r="I12" s="174" t="s">
+      <c r="J12" s="174" t="s">
         <v>333</v>
       </c>
-      <c r="J12" s="174" t="s">
+      <c r="K12" s="174" t="s">
         <v>334</v>
       </c>
-      <c r="K12" s="174" t="s">
+      <c r="L12" s="177" t="s">
         <v>335</v>
-      </c>
-      <c r="L12" s="177" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -4927,7 +4955,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="175" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C13" s="175">
         <f>条件输入!C23</f>
@@ -4975,7 +5003,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="175" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C14" s="175">
         <f>条件输入!C24</f>
@@ -5023,7 +5051,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="175" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C15" s="175">
         <f>条件输入!C25</f>
@@ -5071,7 +5099,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="176" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C16" s="176">
         <f>条件输入!C26</f>
@@ -5118,51 +5146,51 @@
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="121" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B20" s="174" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="243" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D20" s="244"/>
       <c r="E20" s="243" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F20" s="244"/>
       <c r="G20" s="177" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="178"/>
       <c r="B21" s="175"/>
       <c r="C21" s="175" t="s">
+        <v>344</v>
+      </c>
+      <c r="D21" s="175" t="s">
         <v>345</v>
       </c>
-      <c r="D21" s="175" t="s">
-        <v>346</v>
-      </c>
       <c r="E21" s="175" t="s">
+        <v>344</v>
+      </c>
+      <c r="F21" s="175" t="s">
         <v>345</v>
-      </c>
-      <c r="F21" s="175" t="s">
-        <v>346</v>
       </c>
       <c r="G21" s="179"/>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="245" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B22" s="246"/>
       <c r="C22" s="246"/>
@@ -5173,7 +5201,7 @@
     </row>
     <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="178" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B23" s="175"/>
       <c r="C23" s="175">
@@ -5196,7 +5224,7 @@
     </row>
     <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="178" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B24" s="175"/>
       <c r="C24" s="175"/>
@@ -5207,10 +5235,10 @@
     </row>
     <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="178" t="s">
+        <v>349</v>
+      </c>
+      <c r="B25" s="175" t="s">
         <v>350</v>
-      </c>
-      <c r="B25" s="175" t="s">
-        <v>351</v>
       </c>
       <c r="C25" s="175">
         <f>条件输入!C35</f>
@@ -5232,10 +5260,10 @@
     </row>
     <row r="26" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="178" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B26" s="175" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C26" s="175">
         <f>条件输入!C36</f>
@@ -5257,7 +5285,7 @@
     </row>
     <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="245" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B27" s="246"/>
       <c r="C27" s="246"/>
@@ -5268,10 +5296,10 @@
     </row>
     <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="178" t="s">
+        <v>353</v>
+      </c>
+      <c r="B28" s="175" t="s">
         <v>354</v>
-      </c>
-      <c r="B28" s="175" t="s">
-        <v>355</v>
       </c>
       <c r="C28" s="175">
         <f>条件输入!C38</f>
@@ -5293,7 +5321,7 @@
     </row>
     <row r="29" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="178" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B29" s="175"/>
       <c r="C29" s="175">
@@ -5316,7 +5344,7 @@
     </row>
     <row r="30" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="245" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B30" s="246"/>
       <c r="C30" s="246"/>
@@ -5327,7 +5355,7 @@
     </row>
     <row r="31" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="178" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B31" s="175"/>
       <c r="C31" s="175">
@@ -5350,7 +5378,7 @@
     </row>
     <row r="32" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="180" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B32" s="176"/>
       <c r="C32" s="176">
@@ -5375,11 +5403,11 @@
     <row r="34" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B35" s="193"/>
       <c r="C35" s="193" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D35" s="193"/>
       <c r="E35" s="193"/>
@@ -5472,7 +5500,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>5</v>
@@ -5609,10 +5637,10 @@
     </row>
     <row r="49" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C49" s="50" t="s">
         <v>369</v>
-      </c>
-      <c r="C49" s="50" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
@@ -5779,10 +5807,10 @@
     </row>
     <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
@@ -5850,7 +5878,7 @@
         <v>403.82</v>
       </c>
       <c r="E64" s="95" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
@@ -5950,7 +5978,7 @@
         <v>1993.67</v>
       </c>
       <c r="E70" s="95" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
@@ -6193,10 +6221,10 @@
     </row>
     <row r="88" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C88" s="191" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.15">
@@ -6306,7 +6334,7 @@
         <v>4</v>
       </c>
       <c r="B94" s="182" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C94" s="183" t="s">
         <v>99</v>
@@ -6326,7 +6354,7 @@
         <v>5</v>
       </c>
       <c r="B95" s="185" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C95" s="183" t="s">
         <v>101</v>
@@ -6366,7 +6394,7 @@
         <v>7</v>
       </c>
       <c r="B97" s="185" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C97" s="183" t="s">
         <v>5</v>
@@ -6486,7 +6514,7 @@
         <v>4</v>
       </c>
       <c r="B103" s="182" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C103" s="183" t="s">
         <v>99</v>
@@ -6506,7 +6534,7 @@
         <v>5</v>
       </c>
       <c r="B104" s="182" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C104" s="183" t="s">
         <v>99</v>
@@ -6526,7 +6554,7 @@
         <v>6</v>
       </c>
       <c r="B105" s="185" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C105" s="183" t="s">
         <v>101</v>
@@ -6566,7 +6594,7 @@
         <v>8</v>
       </c>
       <c r="B107" s="185" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C107" s="183" t="s">
         <v>5</v>
@@ -6746,7 +6774,7 @@
         <v>5</v>
       </c>
       <c r="B116" s="182" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C116" s="183" t="s">
         <v>99</v>
@@ -6766,7 +6794,7 @@
         <v>6</v>
       </c>
       <c r="B117" s="185" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C117" s="183" t="s">
         <v>101</v>
@@ -6806,7 +6834,7 @@
         <v>8</v>
       </c>
       <c r="B119" s="185" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C119" s="183" t="s">
         <v>5</v>
@@ -7043,10 +7071,10 @@
     </row>
     <row r="133" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C133" s="192" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.15">
@@ -7172,10 +7200,10 @@
     </row>
     <row r="143" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.15">
@@ -7320,10 +7348,10 @@
     </row>
     <row r="153" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.15">
@@ -7331,13 +7359,13 @@
         <v>12</v>
       </c>
       <c r="B154" s="226" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C154" s="226" t="s">
         <v>279</v>
       </c>
       <c r="D154" s="226" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E154" s="226" t="s">
         <v>281</v>
@@ -7380,10 +7408,10 @@
     </row>
     <row r="158" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.15">
@@ -7460,10 +7488,10 @@
     </row>
     <row r="166" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.15">
@@ -7590,11 +7618,11 @@
     </row>
     <row r="178" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B178" s="14"/>
       <c r="C178" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D178" s="14"/>
       <c r="E178" s="14"/>
@@ -7673,7 +7701,7 @@
         <v>273</v>
       </c>
       <c r="C183" s="175" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D183" s="203">
         <f>条件输入!D194</f>
@@ -7686,7 +7714,7 @@
         <v>5</v>
       </c>
       <c r="B184" s="175" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C184" s="175" t="s">
         <v>98</v>
@@ -7797,8 +7825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R523"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C182" sqref="C182"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O194" sqref="O194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -7848,7 +7876,7 @@
         <v>116</v>
       </c>
       <c r="M1" s="138" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="24" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -7878,13 +7906,13 @@
         <v>0.19999999999999996</v>
       </c>
       <c r="M2" s="137" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C3" s="10"/>
       <c r="M3" s="140" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -7907,7 +7935,7 @@
         <v>118</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>68</v>
@@ -7919,15 +7947,15 @@
         <v>202</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M4" s="142" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="241" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B5" s="32">
         <v>5</v>
@@ -7961,16 +7989,16 @@
         <v>2</v>
       </c>
       <c r="M5" s="143" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>310</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>274</v>
@@ -7979,10 +8007,10 @@
         <v>275</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -8023,7 +8051,7 @@
     </row>
     <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="145" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
@@ -8033,30 +8061,30 @@
     </row>
     <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="165" t="s">
+        <v>310</v>
+      </c>
+      <c r="B12" s="166" t="s">
         <v>311</v>
       </c>
-      <c r="B12" s="166" t="s">
+      <c r="C12" s="166" t="s">
         <v>312</v>
       </c>
-      <c r="C12" s="166" t="s">
+      <c r="D12" s="166" t="s">
         <v>313</v>
       </c>
-      <c r="D12" s="166" t="s">
+      <c r="E12" s="166" t="s">
         <v>314</v>
       </c>
-      <c r="E12" s="166" t="s">
+      <c r="F12" s="166" t="s">
         <v>315</v>
       </c>
-      <c r="F12" s="166" t="s">
+      <c r="G12" s="167" t="s">
         <v>316</v>
-      </c>
-      <c r="G12" s="167" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="168" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B13" s="146">
         <v>588.5</v>
@@ -8079,7 +8107,7 @@
     </row>
     <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="168" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B14" s="146">
         <v>803.5</v>
@@ -8102,7 +8130,7 @@
     </row>
     <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="168" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B15" s="146">
         <v>801.79899999999998</v>
@@ -8125,7 +8153,7 @@
     </row>
     <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="168" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B16" s="146">
         <v>1908.0029999999999</v>
@@ -8148,7 +8176,7 @@
     </row>
     <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="168" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B17" s="146">
         <v>345</v>
@@ -8171,7 +8199,7 @@
     </row>
     <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="169" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B18" s="148">
         <v>283.5</v>
@@ -8210,7 +8238,7 @@
     </row>
     <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="145" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -8220,40 +8248,40 @@
     </row>
     <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="159" t="s">
+        <v>325</v>
+      </c>
+      <c r="B22" s="160" t="s">
         <v>326</v>
       </c>
-      <c r="B22" s="160" t="s">
+      <c r="C22" s="160" t="s">
         <v>327</v>
       </c>
-      <c r="C22" s="160" t="s">
+      <c r="D22" s="161" t="s">
+        <v>340</v>
+      </c>
+      <c r="E22" s="160" t="s">
         <v>328</v>
       </c>
-      <c r="D22" s="161" t="s">
-        <v>341</v>
-      </c>
-      <c r="E22" s="160" t="s">
+      <c r="F22" s="160" t="s">
         <v>329</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="G22" s="160" t="s">
         <v>330</v>
       </c>
-      <c r="G22" s="160" t="s">
+      <c r="H22" s="160" t="s">
         <v>331</v>
       </c>
-      <c r="H22" s="160" t="s">
+      <c r="I22" s="160" t="s">
         <v>332</v>
       </c>
-      <c r="I22" s="160" t="s">
+      <c r="J22" s="160" t="s">
         <v>333</v>
       </c>
-      <c r="J22" s="160" t="s">
+      <c r="K22" s="160" t="s">
         <v>334</v>
       </c>
-      <c r="K22" s="160" t="s">
+      <c r="L22" s="162" t="s">
         <v>335</v>
-      </c>
-      <c r="L22" s="162" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -8261,7 +8289,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="151" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C23" s="151">
         <v>3</v>
@@ -8299,7 +8327,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="151" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C24" s="151">
         <v>20</v>
@@ -8337,7 +8365,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="153" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C25" s="151"/>
       <c r="D25" s="151"/>
@@ -8355,7 +8383,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="154" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C26" s="155"/>
       <c r="D26" s="155"/>
@@ -8386,7 +8414,7 @@
     </row>
     <row r="29" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="158" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B29" s="24"/>
       <c r="C29" s="24"/>
@@ -8396,43 +8424,43 @@
     </row>
     <row r="30" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="157" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B30" s="157" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="248" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D30" s="250"/>
       <c r="E30" s="248" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F30" s="250"/>
       <c r="G30" s="157" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="157"/>
       <c r="B31" s="157"/>
       <c r="C31" s="157" t="s">
+        <v>344</v>
+      </c>
+      <c r="D31" s="157" t="s">
         <v>345</v>
       </c>
-      <c r="D31" s="157" t="s">
-        <v>346</v>
-      </c>
       <c r="E31" s="157" t="s">
+        <v>344</v>
+      </c>
+      <c r="F31" s="157" t="s">
         <v>345</v>
-      </c>
-      <c r="F31" s="157" t="s">
-        <v>346</v>
       </c>
       <c r="G31" s="157"/>
     </row>
     <row r="32" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="248" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B32" s="249"/>
       <c r="C32" s="249"/>
@@ -8443,7 +8471,7 @@
     </row>
     <row r="33" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="157" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B33" s="157"/>
       <c r="C33" s="157">
@@ -8462,7 +8490,7 @@
     </row>
     <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="157" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B34" s="157"/>
       <c r="C34" s="157"/>
@@ -8473,10 +8501,10 @@
     </row>
     <row r="35" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="157" t="s">
+        <v>349</v>
+      </c>
+      <c r="B35" s="157" t="s">
         <v>350</v>
-      </c>
-      <c r="B35" s="157" t="s">
-        <v>351</v>
       </c>
       <c r="C35" s="157">
         <v>85.85</v>
@@ -8494,10 +8522,10 @@
     </row>
     <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="157" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B36" s="157" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C36" s="157">
         <v>167.44399999999999</v>
@@ -8515,7 +8543,7 @@
     </row>
     <row r="37" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="248" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B37" s="249"/>
       <c r="C37" s="249"/>
@@ -8526,10 +8554,10 @@
     </row>
     <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="157" t="s">
+        <v>353</v>
+      </c>
+      <c r="B38" s="157" t="s">
         <v>354</v>
-      </c>
-      <c r="B38" s="157" t="s">
-        <v>355</v>
       </c>
       <c r="C38" s="157">
         <v>21.475000000000001</v>
@@ -8547,7 +8575,7 @@
     </row>
     <row r="39" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="157" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B39" s="157"/>
       <c r="C39" s="157">
@@ -8566,7 +8594,7 @@
     </row>
     <row r="40" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="248" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B40" s="249"/>
       <c r="C40" s="249"/>
@@ -8577,7 +8605,7 @@
     </row>
     <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="157" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B41" s="157"/>
       <c r="C41" s="157">
@@ -8596,7 +8624,7 @@
     </row>
     <row r="42" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="157" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B42" s="157"/>
       <c r="C42" s="157">
@@ -8624,7 +8652,7 @@
     <row r="44" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="45" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A45" s="31" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -8870,7 +8898,7 @@
     <row r="59" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="60" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A60" s="31" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
@@ -9519,7 +9547,7 @@
       </c>
       <c r="O101" s="81"/>
       <c r="P101" s="81" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q101" s="42"/>
     </row>
@@ -9854,7 +9882,7 @@
       </c>
       <c r="O110" s="80"/>
       <c r="P110" s="81" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q110" s="43"/>
     </row>
@@ -10025,7 +10053,7 @@
         <v>6000</v>
       </c>
       <c r="E115" s="80">
-        <f t="shared" si="5"/>
+        <f>D115*$E$110</f>
         <v>9000</v>
       </c>
       <c r="F115" s="37"/>
@@ -10303,7 +10331,7 @@
       </c>
       <c r="O122" s="80"/>
       <c r="P122" s="81" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q122" s="43"/>
     </row>
@@ -10790,7 +10818,7 @@
       </c>
       <c r="O135" s="80"/>
       <c r="P135" s="80" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q135" s="37"/>
     </row>
@@ -11082,7 +11110,7 @@
         <v>1</v>
       </c>
       <c r="M146" s="122" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="N146" s="26" t="str">
         <f>"{{"&amp;M146&amp;"_1}}"</f>
@@ -11312,7 +11340,7 @@
         <v>1</v>
       </c>
       <c r="B156" s="116" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C156" s="56">
         <f>E47+E48+E62+E63</f>
@@ -11330,7 +11358,7 @@
         <v>1</v>
       </c>
       <c r="M156" s="116" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="N156" s="56" t="str">
         <f>"{{"&amp;M156&amp;"_开挖}}"</f>
@@ -11464,7 +11492,7 @@
         <v>5</v>
       </c>
       <c r="B160" s="116" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C160" s="117">
         <f>A8</f>
@@ -11482,7 +11510,7 @@
         <v>5</v>
       </c>
       <c r="M160" s="116" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="N160" s="56" t="str">
         <f t="shared" si="16"/>
@@ -11502,7 +11530,7 @@
         <v>6</v>
       </c>
       <c r="B161" s="240" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C161" s="119">
         <f>SUM(C156:C160)</f>
@@ -11520,7 +11548,7 @@
         <v>6</v>
       </c>
       <c r="M161" s="240" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="N161" s="56" t="str">
         <f t="shared" si="16"/>
@@ -11728,7 +11756,7 @@
         <v>3</v>
       </c>
       <c r="B173" s="122" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C173" s="123">
         <f t="array" ref="C173">VLOOKUP($H$5&amp;$I$5&amp;$J$5,IF({1,0},升压站基础数据!A$15:A$30&amp;升压站基础数据!B$15:B$30&amp;升压站基础数据!C$15:C$30,升压站基础数据!G$15:G$30),2,0)</f>
@@ -11741,7 +11769,7 @@
         <v>3</v>
       </c>
       <c r="M173" s="122" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="N173" s="123" t="str">
         <f t="shared" si="21"/>
@@ -11756,7 +11784,7 @@
         <v>4</v>
       </c>
       <c r="B174" s="242" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C174" s="125">
         <f>SUM(C171:C173)</f>
@@ -11770,19 +11798,19 @@
         <v>4</v>
       </c>
       <c r="M174" s="242" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="N174" s="123" t="str">
         <f>"{{"&amp;M174&amp;"_永久用地面积}}"</f>
         <v>{{合计_永久用地面积}}</v>
       </c>
       <c r="O174" s="126" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="175" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="176" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="177" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>265</v>
       </c>
@@ -11799,7 +11827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A178" s="105" t="s">
         <v>85</v>
       </c>
@@ -11816,7 +11844,7 @@
         <v>1</v>
       </c>
       <c r="M178" s="122" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="N178" s="108" t="str">
         <f>"{{"&amp;M178&amp;"_临时用地面积}}"</f>
@@ -11824,12 +11852,12 @@
       </c>
       <c r="O178" s="27"/>
     </row>
-    <row r="179" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A179" s="25">
         <v>1</v>
       </c>
       <c r="B179" s="122" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C179" s="108">
         <f>D151</f>
@@ -11840,7 +11868,7 @@
         <v>2</v>
       </c>
       <c r="M179" s="122" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="N179" s="108" t="str">
         <f t="shared" ref="N179:N185" si="22">"{{"&amp;M179&amp;"_临时用地面积}}"</f>
@@ -11848,12 +11876,12 @@
       </c>
       <c r="O179" s="27"/>
     </row>
-    <row r="180" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A180" s="25">
         <v>2</v>
       </c>
       <c r="B180" s="122" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C180" s="127">
         <f>D2*D136-C171-C172</f>
@@ -11864,7 +11892,7 @@
         <v>3</v>
       </c>
       <c r="M180" s="122" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="N180" s="108" t="str">
         <f t="shared" si="22"/>
@@ -11872,12 +11900,12 @@
       </c>
       <c r="O180" s="27"/>
     </row>
-    <row r="181" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A181" s="25">
         <v>3</v>
       </c>
       <c r="B181" s="122" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C181" s="108">
         <f>E101*2.5*1000+E122*(VLOOKUP($A$5,道路基础数据!$A$16:$AJ$23,36))</f>
@@ -11888,7 +11916,7 @@
         <v>4</v>
       </c>
       <c r="M181" s="122" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="N181" s="108" t="str">
         <f t="shared" si="22"/>
@@ -11896,12 +11924,12 @@
       </c>
       <c r="O181" s="27"/>
     </row>
-    <row r="182" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A182" s="25">
         <v>4</v>
       </c>
       <c r="B182" s="122" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C182" s="108">
         <f>(INT(E161/100000)+1)*10000</f>
@@ -11912,7 +11940,7 @@
         <v>5</v>
       </c>
       <c r="M182" s="122" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="N182" s="108" t="str">
         <f t="shared" si="22"/>
@@ -11920,12 +11948,12 @@
       </c>
       <c r="O182" s="27"/>
     </row>
-    <row r="183" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A183" s="25">
         <v>5</v>
       </c>
       <c r="B183" s="122" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C183" s="108">
         <f>E110*(VLOOKUP($A$5,道路基础数据!$A$16:$AJ$23,36))</f>
@@ -11944,7 +11972,7 @@
       </c>
       <c r="O183" s="27"/>
     </row>
-    <row r="184" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A184" s="25">
         <v>6</v>
       </c>
@@ -11960,7 +11988,7 @@
         <v>7</v>
       </c>
       <c r="M184" s="122" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="N184" s="108" t="str">
         <f t="shared" si="22"/>
@@ -11968,12 +11996,12 @@
       </c>
       <c r="O184" s="27"/>
     </row>
-    <row r="185" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A185" s="25">
         <v>7</v>
       </c>
       <c r="B185" s="122" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C185" s="108">
         <f>D8</f>
@@ -11984,22 +12012,22 @@
         <v>8</v>
       </c>
       <c r="M185" s="242" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="N185" s="108" t="str">
         <f t="shared" si="22"/>
         <v>{{合计_临时用地面积}}</v>
       </c>
       <c r="O185" s="126" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="186" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A186" s="106">
         <v>8</v>
       </c>
       <c r="B186" s="242" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C186" s="128">
         <f>SUM(C179:C185)</f>
@@ -12010,9 +12038,9 @@
         <v>333.2142380256293</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="188" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="189" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="188" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="189" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A189" s="14" t="s">
         <v>285</v>
       </c>
@@ -12020,8 +12048,23 @@
       <c r="C189" s="24"/>
       <c r="D189" s="24"/>
       <c r="E189" s="24"/>
-    </row>
-    <row r="190" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L189" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="M189" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="N189" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="O189" s="107" t="s">
+        <v>286</v>
+      </c>
+      <c r="P189" s="61" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A190" s="121" t="s">
         <v>276</v>
       </c>
@@ -12037,13 +12080,27 @@
       <c r="E190" s="61" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="191" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L190" s="25">
+        <v>1</v>
+      </c>
+      <c r="M190" s="122" t="s">
+        <v>423</v>
+      </c>
+      <c r="N190" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="O190" s="108" t="str">
+        <f>"{{"&amp;M190&amp;"_主要施工工程量}}"</f>
+        <v>{{风机机组_主要施工工程量}}</v>
+      </c>
+      <c r="P190" s="27"/>
+    </row>
+    <row r="191" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A191" s="25">
         <v>1</v>
       </c>
-      <c r="B191" s="26" t="s">
-        <v>287</v>
+      <c r="B191" s="122" t="s">
+        <v>423</v>
       </c>
       <c r="C191" s="26" t="s">
         <v>288</v>
@@ -12053,13 +12110,27 @@
         <v>15</v>
       </c>
       <c r="E191" s="27"/>
-    </row>
-    <row r="192" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L191" s="25">
+        <v>2</v>
+      </c>
+      <c r="M191" s="122" t="s">
+        <v>420</v>
+      </c>
+      <c r="N191" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="O191" s="108" t="str">
+        <f t="shared" ref="O191:O199" si="23">"{{"&amp;M191&amp;"_主要施工工程量}}"</f>
+        <v>{{建筑面积_主要施工工程量}}</v>
+      </c>
+      <c r="P191" s="27"/>
+    </row>
+    <row r="192" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A192" s="25">
         <v>2</v>
       </c>
-      <c r="B192" s="26" t="s">
-        <v>289</v>
+      <c r="B192" s="122" t="s">
+        <v>420</v>
       </c>
       <c r="C192" s="26" t="s">
         <v>290</v>
@@ -12069,13 +12140,27 @@
         <v>2197.2399999999998</v>
       </c>
       <c r="E192" s="27"/>
-    </row>
-    <row r="193" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L192" s="25">
+        <v>3</v>
+      </c>
+      <c r="M192" s="122" t="s">
+        <v>424</v>
+      </c>
+      <c r="N192" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="O192" s="108" t="str">
+        <f t="shared" si="23"/>
+        <v>{{主变压器_主要施工工程量}}</v>
+      </c>
+      <c r="P192" s="27"/>
+    </row>
+    <row r="193" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A193" s="25">
         <v>3</v>
       </c>
-      <c r="B193" s="26" t="s">
-        <v>291</v>
+      <c r="B193" s="122" t="s">
+        <v>424</v>
       </c>
       <c r="C193" s="26" t="s">
         <v>288</v>
@@ -12085,45 +12170,87 @@
         <v>2</v>
       </c>
       <c r="E193" s="27"/>
-    </row>
-    <row r="194" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L193" s="25">
+        <v>4</v>
+      </c>
+      <c r="M193" s="122" t="s">
+        <v>273</v>
+      </c>
+      <c r="N193" s="122" t="s">
+        <v>298</v>
+      </c>
+      <c r="O193" s="108" t="str">
+        <f t="shared" si="23"/>
+        <v>{{架空线路_主要施工工程量}}</v>
+      </c>
+      <c r="P193" s="27"/>
+    </row>
+    <row r="194" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A194" s="25">
         <v>4</v>
       </c>
       <c r="B194" s="122" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
       <c r="C194" s="122" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D194" s="108">
         <f>E8</f>
         <v>20</v>
       </c>
       <c r="E194" s="27"/>
-    </row>
-    <row r="195" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L194" s="25">
+        <v>5</v>
+      </c>
+      <c r="M194" s="122" t="s">
+        <v>296</v>
+      </c>
+      <c r="N194" s="122" t="s">
+        <v>98</v>
+      </c>
+      <c r="O194" s="108" t="str">
+        <f t="shared" si="23"/>
+        <v>{{直埋电缆_主要施工工程量}}</v>
+      </c>
+      <c r="P194" s="27"/>
+    </row>
+    <row r="195" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A195" s="25">
         <v>5</v>
       </c>
       <c r="B195" s="122" t="s">
+        <v>296</v>
+      </c>
+      <c r="C195" s="122" t="s">
         <v>297</v>
-      </c>
-      <c r="C195" s="122" t="s">
-        <v>298</v>
       </c>
       <c r="D195" s="108">
         <f>F8</f>
         <v>2</v>
       </c>
       <c r="E195" s="27"/>
-    </row>
-    <row r="196" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L195" s="25">
+        <v>6</v>
+      </c>
+      <c r="M195" s="122" t="s">
+        <v>421</v>
+      </c>
+      <c r="N195" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="O195" s="108" t="str">
+        <f t="shared" si="23"/>
+        <v>{{土石方开挖_主要施工工程量}}</v>
+      </c>
+      <c r="P195" s="27"/>
+    </row>
+    <row r="196" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A196" s="25">
         <v>6</v>
       </c>
-      <c r="B196" s="26" t="s">
-        <v>292</v>
+      <c r="B196" s="122" t="s">
+        <v>421</v>
       </c>
       <c r="C196" s="26" t="s">
         <v>293</v>
@@ -12133,13 +12260,27 @@
         <v>35.491470666084133</v>
       </c>
       <c r="E196" s="27"/>
-    </row>
-    <row r="197" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L196" s="25">
+        <v>7</v>
+      </c>
+      <c r="M196" s="122" t="s">
+        <v>425</v>
+      </c>
+      <c r="N196" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="O196" s="108" t="str">
+        <f t="shared" si="23"/>
+        <v>{{土石方回填_主要施工工程量}}</v>
+      </c>
+      <c r="P196" s="27"/>
+    </row>
+    <row r="197" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A197" s="25">
         <v>7</v>
       </c>
-      <c r="B197" s="26" t="s">
-        <v>7</v>
+      <c r="B197" s="122" t="s">
+        <v>425</v>
       </c>
       <c r="C197" s="26" t="s">
         <v>293</v>
@@ -12149,13 +12290,27 @@
         <v>10.173111605807936</v>
       </c>
       <c r="E197" s="27"/>
-    </row>
-    <row r="198" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L197" s="25">
+        <v>8</v>
+      </c>
+      <c r="M197" s="122" t="s">
+        <v>426</v>
+      </c>
+      <c r="N197" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="O197" s="108" t="str">
+        <f t="shared" si="23"/>
+        <v>{{混凝土_主要施工工程量}}</v>
+      </c>
+      <c r="P197" s="27"/>
+    </row>
+    <row r="198" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A198" s="25">
         <v>8</v>
       </c>
-      <c r="B198" s="26" t="s">
-        <v>294</v>
+      <c r="B198" s="122" t="s">
+        <v>426</v>
       </c>
       <c r="C198" s="26" t="s">
         <v>293</v>
@@ -12165,13 +12320,27 @@
         <v>1.2135933102761951</v>
       </c>
       <c r="E198" s="27"/>
-    </row>
-    <row r="199" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L198" s="25">
+        <v>9</v>
+      </c>
+      <c r="M198" s="122" t="s">
+        <v>427</v>
+      </c>
+      <c r="N198" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="O198" s="108" t="str">
+        <f t="shared" si="23"/>
+        <v>{{钢筋_主要施工工程量}}</v>
+      </c>
+      <c r="P198" s="27"/>
+    </row>
+    <row r="199" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A199" s="25">
         <v>9</v>
       </c>
-      <c r="B199" s="26" t="s">
-        <v>9</v>
+      <c r="B199" s="122" t="s">
+        <v>427</v>
       </c>
       <c r="C199" s="26" t="s">
         <v>10</v>
@@ -12181,13 +12350,27 @@
         <v>919.21037699350632</v>
       </c>
       <c r="E199" s="27"/>
-    </row>
-    <row r="200" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="L199" s="106">
+        <v>10</v>
+      </c>
+      <c r="M199" s="242" t="s">
+        <v>422</v>
+      </c>
+      <c r="N199" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="O199" s="108" t="str">
+        <f t="shared" si="23"/>
+        <v>{{浆砌石_主要施工工程量}}</v>
+      </c>
+      <c r="P199" s="30"/>
+    </row>
+    <row r="200" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A200" s="106">
         <v>10</v>
       </c>
-      <c r="B200" s="29" t="s">
-        <v>295</v>
+      <c r="B200" s="242" t="s">
+        <v>422</v>
       </c>
       <c r="C200" s="29" t="s">
         <v>293</v>
@@ -12198,14 +12381,14 @@
       </c>
       <c r="E200" s="30"/>
     </row>
-    <row r="201" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="202" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="203" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="204" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="205" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="206" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="207" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="208" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="201" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="202" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="203" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="204" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="205" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="206" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="207" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="208" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="209" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="210" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="211" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>